<commit_message>
Box and Molecules class
</commit_message>
<xml_diff>
--- a/Requirements Register.xlsx
+++ b/Requirements Register.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduumb-my.sharepoint.com/personal/le_uyen_nhu_dinh_nmbu_no/Documents/June Block/INF203/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A68C3771-4D18-BC43-B69A-1B090A904C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D706D5B-9900-2D46-80CC-1D12871A70DF}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{A68C3771-4D18-BC43-B69A-1B090A904C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EF83992-ED1B-3642-BE6D-96622C5AAB13}"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="9500" windowWidth="28040" windowHeight="17160" xr2:uid="{FC6790B6-D8BC-5941-80A3-06560992F1E7}"/>
+    <workbookView xWindow="2900" yWindow="3580" windowWidth="28040" windowHeight="17160" xr2:uid="{FC6790B6-D8BC-5941-80A3-06560992F1E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Epic</t>
+  </si>
+  <si>
+    <t>User Story</t>
+  </si>
+  <si>
+    <t>Persona</t>
+  </si>
+  <si>
+    <t>Priority (MoSCoW)</t>
   </si>
 </sst>
 </file>
@@ -62,7 +71,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,12 +79,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,18 +438,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34674974-40F5-5140-98C6-5D80199ACDC2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix distance function with correct PBC
</commit_message>
<xml_diff>
--- a/Requirements Register.xlsx
+++ b/Requirements Register.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduumb-my.sharepoint.com/personal/le_uyen_nhu_dinh_nmbu_no/Documents/June Block/INF203/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{A68C3771-4D18-BC43-B69A-1B090A904C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EF83992-ED1B-3642-BE6D-96622C5AAB13}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="8_{A68C3771-4D18-BC43-B69A-1B090A904C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EC75A68-8929-0542-BE0D-7884EA4EACBF}"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="3580" windowWidth="28040" windowHeight="17160" xr2:uid="{FC6790B6-D8BC-5941-80A3-06560992F1E7}"/>
+    <workbookView xWindow="11720" yWindow="720" windowWidth="17680" windowHeight="18400" xr2:uid="{FC6790B6-D8BC-5941-80A3-06560992F1E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,25 +36,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Epic</t>
-  </si>
-  <si>
-    <t>User Story</t>
-  </si>
-  <si>
-    <t>Persona</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Priority (MoSCoW)</t>
+  </si>
+  <si>
+    <t>Personas</t>
+  </si>
+  <si>
+    <t>Epics</t>
+  </si>
+  <si>
+    <t>User Stories</t>
+  </si>
+  <si>
+    <t>Simulation Sofware Developer</t>
+  </si>
+  <si>
+    <t>Computational Physicist</t>
+  </si>
+  <si>
+    <t>Calculation of Surface Tension using Test-Area Method</t>
+  </si>
+  <si>
+    <t>I want to implement the Test-Area Method for planar interfaces so that I can evaluate mechanical model predictions.</t>
+  </si>
+  <si>
+    <t>Must</t>
+  </si>
+  <si>
+    <t>Should</t>
+  </si>
+  <si>
+    <t>Won't</t>
+  </si>
+  <si>
+    <t>Could</t>
+  </si>
+  <si>
+    <t>I want to apply Test-Area deformations to spherical droplets to observe fluctuation effects on surface tension.</t>
+  </si>
+  <si>
+    <t>Energy Fluctuation Analysis</t>
+  </si>
+  <si>
+    <t>Research Data Analyst</t>
+  </si>
+  <si>
+    <t>I want to analyse the first-, second-, third-order energy contributions to compute the free energy.</t>
+  </si>
+  <si>
+    <t>Performance of The Simulations</t>
+  </si>
+  <si>
+    <t>Physics Student</t>
+  </si>
+  <si>
+    <t>I want to visualize 3D fluctuations in real-time</t>
+  </si>
+  <si>
+    <t>I want to optimize the execution of  the molecule dynamic to reduce the computation time for complex simulation.</t>
+  </si>
+  <si>
+    <t>I want the simulation software to visualize and compute correctly the nanoscale droplet behaviour with the provided configuration on the 3D cuboid.</t>
+  </si>
+  <si>
+    <t>I want to develop statiscal modules to distinguish Gaussian distribution behaviors of energy fluctuations.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -62,16 +116,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -94,16 +161,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -119,6 +232,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,68 +555,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34674974-40F5-5140-98C6-5D80199ACDC2}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="28" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+    </row>
+    <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A8"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1" xr:uid="{CF87FB63-F991-464C-9D56-8C74E16EBF6B}">
+      <formula1>$G$2:$G$5</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add epics to Requirement Register
</commit_message>
<xml_diff>
--- a/Requirements Register.xlsx
+++ b/Requirements Register.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduumb-my.sharepoint.com/personal/le_uyen_nhu_dinh_nmbu_no/Documents/June Block/INF203/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="8_{A68C3771-4D18-BC43-B69A-1B090A904C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EC75A68-8929-0542-BE0D-7884EA4EACBF}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="8_{A68C3771-4D18-BC43-B69A-1B090A904C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A12C282-28CA-344F-B10B-5210FB9A8F02}"/>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="720" windowWidth="17680" windowHeight="18400" xr2:uid="{FC6790B6-D8BC-5941-80A3-06560992F1E7}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{FC6790B6-D8BC-5941-80A3-06560992F1E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Priority (MoSCoW)</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Calculation of Surface Tension using Test-Area Method</t>
   </si>
   <si>
-    <t>I want to implement the Test-Area Method for planar interfaces so that I can evaluate mechanical model predictions.</t>
-  </si>
-  <si>
     <t>Must</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>Energy Fluctuation Analysis</t>
   </si>
   <si>
-    <t>Research Data Analyst</t>
-  </si>
-  <si>
     <t>I want to analyse the first-, second-, third-order energy contributions to compute the free energy.</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t>Physics Student</t>
   </si>
   <si>
-    <t>I want to visualize 3D fluctuations in real-time</t>
-  </si>
-  <si>
     <t>I want to optimize the execution of  the molecule dynamic to reduce the computation time for complex simulation.</t>
   </si>
   <si>
@@ -102,13 +93,40 @@
   </si>
   <si>
     <t>I want to develop statiscal modules to distinguish Gaussian distribution behaviors of energy fluctuations.</t>
+  </si>
+  <si>
+    <t>I want to implement the Test-Area Method for both planar and spherical interfaces so that I can evaluate mechanical model predictions.</t>
+  </si>
+  <si>
+    <t>I want to visualize 3D energy changes in real-time</t>
+  </si>
+  <si>
+    <t>Research Analyst</t>
+  </si>
+  <si>
+    <t>Implementation of Monte Carlo Methodology in Computation</t>
+  </si>
+  <si>
+    <t>Simulation Software Developer</t>
+  </si>
+  <si>
+    <t>I want to implement Monte Carlo method (Metropolis algorithms) to sample configuration efficiently for small droplets.</t>
+  </si>
+  <si>
+    <t>I want to compare Monte Carlo results with molecular dynamics to validate free energy computations.</t>
+  </si>
+  <si>
+    <t>I want to understand and visualize how probabilistic sampling affects the predicted properties of nanoscale systems.</t>
+  </si>
+  <si>
+    <t>I want to generate comparative plots between Monte Carlo and traditional methods to present in reports.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -121,6 +139,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -191,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -202,7 +227,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -211,12 +239,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,130 +581,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34674974-40F5-5140-98C6-5D80199ACDC2}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="36.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="4" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
+    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A12"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1" xr:uid="{CF87FB63-F991-464C-9D56-8C74E16EBF6B}">

</xml_diff>